<commit_message>
adding courses by dow
</commit_message>
<xml_diff>
--- a/inputs/Course_Catalog_Reviewed.xlsx
+++ b/inputs/Course_Catalog_Reviewed.xlsx
@@ -1,33 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/claudiasatterfield/Dev/Scholacity_Parser/Scholacity_Parser/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA8C3D97-9A0D-F844-B589-BA37205F220F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31C80E33-215F-4545-BCB7-ED9BCE03BAD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25240" yWindow="3680" windowWidth="28080" windowHeight="17080" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18560" yWindow="4260" windowWidth="28080" windowHeight="17080" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Courses" sheetId="1" r:id="rId1"/>
     <sheet name="Sessions" sheetId="8" r:id="rId2"/>
-    <sheet name="Arts and Literature" sheetId="2" r:id="rId3"/>
-    <sheet name="Business, Finance and Technolog" sheetId="3" r:id="rId4"/>
-    <sheet name="Culture, Travel and Tours" sheetId="4" r:id="rId5"/>
-    <sheet name="Gardening and Environment" sheetId="5" r:id="rId6"/>
-    <sheet name="History and Current Affairs" sheetId="6" r:id="rId7"/>
-    <sheet name="Science and Health" sheetId="7" r:id="rId8"/>
+    <sheet name="Courses_DOW" sheetId="11" r:id="rId3"/>
+    <sheet name="Arts and Literature" sheetId="2" r:id="rId4"/>
+    <sheet name="Business, Finance and Technolog" sheetId="3" r:id="rId5"/>
+    <sheet name="Culture, Travel and Tours" sheetId="4" r:id="rId6"/>
+    <sheet name="Gardening and Environment" sheetId="5" r:id="rId7"/>
+    <sheet name="History and Current Affairs" sheetId="6" r:id="rId8"/>
+    <sheet name="Science and Health" sheetId="7" r:id="rId9"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="290">
   <si>
     <t>LearningObjective</t>
   </si>
@@ -903,7 +904,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -939,6 +940,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -961,7 +969,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -976,6 +984,8 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2171,10 +2181,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A497878-9AC6-C64D-BF5E-F9407587F5F1}">
   <dimension ref="A1:H80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="B77" sqref="B77"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4284,6 +4294,507 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{728CF261-AAB8-4B41-8056-4B261A2FEA52}">
+  <dimension ref="A1:C43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="61.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>289</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:I43">
+    <sortCondition ref="A1:A43"/>
+    <sortCondition ref="C1:C43"/>
+  </sortState>
+  <hyperlinks>
+    <hyperlink ref="B28" r:id="rId1" display="https://console.firebase.google.com/u/0/project/scholacity-org/database/scholacity-org/data/course/-MJD-ku1_KeDsaiQlRkl" xr:uid="{2F217C82-59CD-1746-A0BB-D59A6F23B218}"/>
+    <hyperlink ref="B29" r:id="rId2" display="https://console.firebase.google.com/u/0/project/scholacity-org/database/scholacity-org/data/course/-MJD-kwnSHCYasZfzRZE" xr:uid="{93B993F1-46CE-6945-9178-4459004768A4}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E17"/>
   <sheetViews>
@@ -4546,7 +5057,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E13"/>
   <sheetViews>
@@ -4753,7 +5264,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -4820,7 +5331,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
@@ -4985,7 +5496,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E14"/>
   <sheetViews>
@@ -5206,7 +5717,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E13"/>
   <sheetViews>

</xml_diff>